<commit_message>
Sync old Cornell laptop 13 Sept 2024
</commit_message>
<xml_diff>
--- a/outputs/result_37pct_comparison_spp_names_RAN.xlsx
+++ b/outputs/result_37pct_comparison_spp_names_RAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raenb\Documents\GitHub\es_birds_usa\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C0D19E1E-1602-42FE-B760-049D1C54EAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC134FB-65EE-4043-9452-552E7B35F5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result_37pct_comparison_spp_nam" sheetId="1" r:id="rId1"/>
@@ -4401,7 +4401,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -5250,7 +5250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23517,7 +23517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L480"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41776,7 +41776,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:I480"/>
+  <autoFilter ref="H1:I480" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L480">
     <sortCondition descending="1" ref="J2:J480"/>
   </sortState>
@@ -41785,12 +41785,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T480"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61:XFD61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>